<commit_message>
envoie de mes fichiers
</commit_message>
<xml_diff>
--- a/test_unitaire.xlsx
+++ b/test_unitaire.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -37,16 +37,10 @@
     <t>Produit.js</t>
   </si>
   <si>
-    <t>document.getElementById</t>
-  </si>
-  <si>
     <t>itemAdd</t>
   </si>
   <si>
     <t>panier.js</t>
-  </si>
-  <si>
-    <t>recap.js</t>
   </si>
   <si>
     <t>produit.js</t>
@@ -74,9 +68,6 @@
   </si>
   <si>
     <t xml:space="preserve">afficher le produit sans ces options dans le panier </t>
-  </si>
-  <si>
-    <t>49 à 54</t>
   </si>
   <si>
     <t>ajoutez le produit au panier pour voir si elle fonctionne</t>
@@ -115,31 +106,16 @@
     <t>Total de la commande</t>
   </si>
   <si>
-    <t>Tester en dur avec des valeurs differentes. Ajoutez l'element dans panier pour tester</t>
-  </si>
-  <si>
     <t>certains éléments pourraient ne pas être selectionnés</t>
   </si>
   <si>
     <t>parier</t>
   </si>
   <si>
-    <t>La fonction (asynchrone) appelle la methode fetch() qui lance une requête afin de récupérer une promesse : la réponse est un object et cette donnée est accessible via la méthode json()</t>
-  </si>
-  <si>
-    <t>async</t>
-  </si>
-  <si>
     <t>38 à 40</t>
   </si>
   <si>
-    <t>Tester l'URL avec un client HTTP pour vérifier le retour du serveur</t>
-  </si>
-  <si>
     <t>Aucune réponse du serveur =&gt; Url (route) incorrecte</t>
-  </si>
-  <si>
-    <t>85 à 109</t>
   </si>
   <si>
     <t>Envoyer les données du formulaire et le tableau des articles dans le panier à l'API</t>
@@ -150,12 +126,48 @@
   <si>
     <t>Vérification dans la console des élements envoyer par route Post au backend</t>
   </si>
+  <si>
+    <t>101 à 138</t>
+  </si>
+  <si>
+    <t>sendData</t>
+  </si>
+  <si>
+    <t>47 à 54</t>
+  </si>
+  <si>
+    <t>La fonction (getOrderId) appelle la methode fetch() qui lance une requête afin de récupérer une promesse : la réponse est un object et cette donnée est accessible via la méthode json()</t>
+  </si>
+  <si>
+    <t>isInvalid</t>
+  </si>
+  <si>
+    <t>getOrderId</t>
+  </si>
+  <si>
+    <t>42 à 99</t>
+  </si>
+  <si>
+    <t>Elle verifie les expressions utilisés dans les champs du formilaire. Exemple pas de chiffre dans le champ prénon</t>
+  </si>
+  <si>
+    <t>Testez en dur avec des valeurs differentes. Ajoutez l'element dans panier pour tester</t>
+  </si>
+  <si>
+    <t>Testez l'URL avec un client HTTP pour vérifier le retour du serveur</t>
+  </si>
+  <si>
+    <t>Passer la commande sans effectuer les vérifications des données du formulaire lors du clic sur le bouton « passer commande »</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testez le en dur, mettez des chiffres dans les champs prénom, nom ou ville </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -201,6 +213,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -228,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -287,6 +304,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,42 +597,42 @@
     </row>
     <row r="3" spans="1:26" ht="61.5" customHeight="1">
       <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="E3" s="12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="61.5" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="76.5" customHeight="1">
@@ -617,111 +640,125 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="61.5" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="61.5" customHeight="1">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="66" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="50.25" customHeight="1">
+      <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>23</v>
+      <c r="B9" s="22" t="s">
+        <v>43</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
+      <c r="C9" s="21" t="s">
+        <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" ht="61.5" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>25</v>
+      <c r="D9" s="2" t="s">
+        <v>44</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
+      <c r="E9" s="2" t="s">
+        <v>48</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>27</v>
+      <c r="F9" s="2" t="s">
+        <v>47</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>28</v>
+    </row>
+    <row r="10" spans="1:26" ht="61.5" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>29</v>
+      <c r="B10" s="3" t="s">
+        <v>37</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>30</v>
+      <c r="C10" s="15" t="s">
+        <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" ht="61.5" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="20" t="s">
+      <c r="D10" s="15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" ht="61.5" customHeight="1">
-      <c r="A8" s="3" t="s">
+      <c r="E10" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="61.5" customHeight="1">
-      <c r="A9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="61.5" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="61.5" customHeight="1">
+      <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="14"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="15"/>

</xml_diff>